<commit_message>
update init values for benthic LTL
</commit_message>
<xml_diff>
--- a/NEUS_v15_Initial_Biomass.xlsx
+++ b/NEUS_v15_Initial_Biomass.xlsx
@@ -266,9 +266,6 @@
     <t>ISQ</t>
   </si>
   <si>
-    <t>NEUS v1.0 40% of parent</t>
-  </si>
-  <si>
     <t>SCA</t>
   </si>
   <si>
@@ -675,6 +672,9 @@
   </si>
   <si>
     <t>Mean seasonal values from D. Townsend</t>
+  </si>
+  <si>
+    <t>Double trawl suvey non_Q corrected timeseries mean (no reliable published values)</t>
   </si>
 </sst>
 </file>
@@ -719,12 +719,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="53.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,10 +1026,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1039,7 +1040,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="1">
         <v>6637.5</v>
@@ -1053,7 +1054,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" s="1">
         <v>4510.6719999999996</v>
@@ -1067,7 +1068,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="1">
         <v>80218.806890000007</v>
@@ -1081,7 +1082,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="1">
         <v>2697</v>
@@ -1095,7 +1096,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6" s="1">
         <v>12347.108630000001</v>
@@ -1109,7 +1110,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C7" s="1">
         <v>3907.9740299999999</v>
@@ -1123,7 +1124,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" s="1">
         <v>35892.089209999998</v>
@@ -1137,7 +1138,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" s="1">
         <v>21423.01856</v>
@@ -1151,7 +1152,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C10" s="1">
         <v>8105.2905899999996</v>
@@ -1165,7 +1166,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C11" s="1">
         <v>3646.2221399999999</v>
@@ -1179,7 +1180,7 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C12" s="1">
         <v>38854.992890000001</v>
@@ -1193,13 +1194,13 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C13" s="1">
         <v>657</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1207,7 +1208,7 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" s="1">
         <v>1596.4079999999999</v>
@@ -1221,7 +1222,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" s="1">
         <v>2273.672</v>
@@ -1235,7 +1236,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" s="1">
         <v>967.52</v>
@@ -1249,13 +1250,13 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" s="1">
         <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1263,7 +1264,7 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" s="1">
         <v>5673.2709999999997</v>
@@ -1277,7 +1278,7 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" s="1">
         <v>12508.14644</v>
@@ -1291,7 +1292,7 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="1">
         <v>2343.3339999999998</v>
@@ -1305,7 +1306,7 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C21" s="1">
         <v>66381.201029999997</v>
@@ -1319,7 +1320,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C22" s="1">
         <v>3164.95</v>
@@ -1333,7 +1334,7 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C23" s="1">
         <v>4742.7510000000002</v>
@@ -1347,7 +1348,7 @@
         <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C24" s="1">
         <v>312490.47648000001</v>
@@ -1361,7 +1362,7 @@
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C25" s="1">
         <v>124595.38234</v>
@@ -1375,7 +1376,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C26" s="1">
         <v>639.21481000000006</v>
@@ -1389,7 +1390,7 @@
         <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C27" s="1">
         <v>247495.45460999999</v>
@@ -1403,7 +1404,7 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C28" s="1">
         <v>68851.370939999993</v>
@@ -1417,7 +1418,7 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C29" s="1">
         <v>858.70898</v>
@@ -1431,7 +1432,7 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C30" s="1">
         <v>8099.2672199999997</v>
@@ -1445,7 +1446,7 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C31" s="1">
         <v>466.91953999999998</v>
@@ -1459,7 +1460,7 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C32" s="1">
         <v>204570.50472</v>
@@ -1473,7 +1474,7 @@
         <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C33" s="1">
         <v>68242.971520000006</v>
@@ -1487,7 +1488,7 @@
         <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C34" s="1">
         <v>26.160060000000001</v>
@@ -1501,7 +1502,7 @@
         <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C35" s="1">
         <v>444.32128</v>
@@ -1515,7 +1516,7 @@
         <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C36" s="1">
         <v>2041.1949999999999</v>
@@ -1529,7 +1530,7 @@
         <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C37" s="1">
         <v>385.52397999999999</v>
@@ -1543,7 +1544,7 @@
         <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C38" s="1">
         <v>6193.6677499999996</v>
@@ -1557,7 +1558,7 @@
         <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C39" s="1">
         <v>638.52646000000004</v>
@@ -1571,7 +1572,7 @@
         <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C40" s="1">
         <v>287990.48550000001</v>
@@ -1585,7 +1586,7 @@
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C41" s="1">
         <v>837622.32530000003</v>
@@ -1599,7 +1600,7 @@
         <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C42" s="1">
         <v>88958.136549999996</v>
@@ -1613,7 +1614,7 @@
         <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C43" s="1">
         <v>633208.32400000002</v>
@@ -1627,7 +1628,7 @@
         <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C44" s="1">
         <v>17226.46154</v>
@@ -1641,7 +1642,7 @@
         <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C45" s="1">
         <v>3484.8640300000002</v>
@@ -1655,7 +1656,7 @@
         <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C46" s="1">
         <v>1253.7247</v>
@@ -1669,7 +1670,7 @@
         <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C47" s="1">
         <v>2873.4</v>
@@ -1683,7 +1684,7 @@
         <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C48" s="1">
         <v>1436.7</v>
@@ -1697,7 +1698,7 @@
         <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C49" s="1">
         <v>3114.6878999999999</v>
@@ -1711,7 +1712,7 @@
         <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C50" s="1">
         <v>128678.71575</v>
@@ -1725,7 +1726,7 @@
         <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C51" s="1">
         <v>130790.82432</v>
@@ -1739,7 +1740,7 @@
         <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C52" s="1">
         <v>181995.72683</v>
@@ -1753,7 +1754,7 @@
         <v>65</v>
       </c>
       <c r="B53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C53" s="1">
         <v>1808.5</v>
@@ -1767,7 +1768,7 @@
         <v>67</v>
       </c>
       <c r="B54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C54" s="1">
         <v>7660.8</v>
@@ -1781,7 +1782,7 @@
         <v>68</v>
       </c>
       <c r="B55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C55" s="1">
         <v>803.2</v>
@@ -1795,7 +1796,7 @@
         <v>69</v>
       </c>
       <c r="B56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C56" s="1">
         <v>18046.14</v>
@@ -1809,7 +1810,7 @@
         <v>71</v>
       </c>
       <c r="B57" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C57" s="1">
         <v>72184.56</v>
@@ -1823,7 +1824,7 @@
         <v>73</v>
       </c>
       <c r="B58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C58" s="1">
         <v>11998.44</v>
@@ -1837,7 +1838,7 @@
         <v>75</v>
       </c>
       <c r="B59" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C59" s="1">
         <v>7998.96</v>
@@ -1851,7 +1852,7 @@
         <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C60" s="1">
         <v>2616.0059999999999</v>
@@ -1865,13 +1866,13 @@
         <v>78</v>
       </c>
       <c r="B61" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C61" s="1">
         <v>27578</v>
       </c>
       <c r="D61" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1879,77 +1880,77 @@
         <v>79</v>
       </c>
       <c r="B62" t="s">
-        <v>178</v>
-      </c>
-      <c r="C62" s="1">
-        <v>29746.28</v>
+        <v>177</v>
+      </c>
+      <c r="C62" s="5">
+        <v>10000</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>80</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B63" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C63" s="1">
         <v>35183</v>
       </c>
       <c r="D63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C64" s="4">
         <v>3178000</v>
       </c>
       <c r="D64" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C65" s="1">
         <v>1000000</v>
       </c>
       <c r="D65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B66" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C66" s="1">
         <v>1540650.925</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B67" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C67" s="1">
         <v>5035438.5999999996</v>
@@ -1960,10 +1961,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B68" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C68" s="1">
         <v>20570</v>
@@ -1974,80 +1975,80 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B69" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C69" s="1">
         <v>434</v>
       </c>
       <c r="D69" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C70" s="1">
         <v>723132.18</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B71" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C71" s="1">
         <v>45000</v>
       </c>
       <c r="D71" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B72" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C72" s="1">
         <v>90000</v>
       </c>
       <c r="D72" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B73" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C73" s="1">
         <v>88497.144625719302</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B74" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C74" s="1">
         <v>375230138.30000001</v>
@@ -2058,52 +2059,52 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B75" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C75" s="3">
         <v>53524.93</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B76" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C76" s="1">
         <v>0</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B77" t="s">
         <v>199</v>
-      </c>
-      <c r="B77" t="s">
-        <v>200</v>
       </c>
       <c r="C77" s="3">
         <v>20571.62</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B78" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C78" s="1">
         <v>6025037.2999999998</v>
@@ -2114,94 +2115,94 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B79" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C79" s="1">
         <v>151644.371947782</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B80" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C80" s="1">
         <v>548371.06777746405</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B81" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C81" s="1">
         <v>201134.73789574299</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B82" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C82" s="1">
         <v>163315.90861250801</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C83" s="1">
         <v>94440.610721329402</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C84" s="1">
         <v>374087.87270517001</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B85" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C85" s="1">
         <v>31842.799999999999</v>
@@ -2212,10 +2213,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B86" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C86" s="1">
         <v>15062593.300000001</v>
@@ -2226,10 +2227,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C87" s="1">
         <v>60250373.299999997</v>
@@ -2240,10 +2241,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C88" s="3">
         <v>15052390</v>
@@ -2254,10 +2255,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B89" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C89" s="3">
         <v>60209.57</v>
@@ -2268,30 +2269,30 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B90" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C90" s="1">
         <v>0</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B91" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C91" s="3">
         <v>329358000</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
scale HER to match SAW 65th report values for biomass in 1965
</commit_message>
<xml_diff>
--- a/NEUS_v15_Initial_Biomass.xlsx
+++ b/NEUS_v15_Initial_Biomass.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="218">
   <si>
     <t>Code</t>
   </si>
@@ -675,6 +675,9 @@
   </si>
   <si>
     <t>Double trawl suvey non_Q corrected timeseries mean (no reliable published values)</t>
+  </si>
+  <si>
+    <t>65th SAW report ASAP model estimate Jan 1, p440, Table B4-2</t>
   </si>
 </sst>
 </file>
@@ -1008,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="53.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,10 +1060,10 @@
         <v>115</v>
       </c>
       <c r="C3" s="1">
-        <v>4510.6719999999996</v>
+        <v>1684170</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>